<commit_message>
update casos de prueba
</commit_message>
<xml_diff>
--- a/Fase_1/Evidencias_Grupales/Plantilla Casos de prueba Integracion.xlsx
+++ b/Fase_1/Evidencias_Grupales/Plantilla Casos de prueba Integracion.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="93">
   <si>
     <t>UnidadTerritorial</t>
   </si>
@@ -185,10 +185,31 @@
     <t>CA005</t>
   </si>
   <si>
+    <t>Sistema de registro de usuario</t>
+  </si>
+  <si>
+    <t>Se harán pruebas de la funcionalidad de registro de usuario</t>
+  </si>
+  <si>
+    <t>Datos de usuario registrado, conexión a base de datos</t>
+  </si>
+  <si>
     <t>CA006</t>
   </si>
   <si>
+    <t>Sistema de inicio de sesión</t>
+  </si>
+  <si>
+    <t>Se harán pruebas de la funcionalidad de inicio de sesióm</t>
+  </si>
+  <si>
     <t>CA007</t>
+  </si>
+  <si>
+    <t>Sistema de gestión de usuarios</t>
+  </si>
+  <si>
+    <t>Se harán pruebas de la funcionalidad de gestión de usuarios</t>
   </si>
   <si>
     <t>CA008</t>
@@ -240,6 +261,66 @@
   </si>
   <si>
     <t>Al cancelar la reserva debe habilitarse la opción de reserva que estaba deshabilitada</t>
+  </si>
+  <si>
+    <t>Ingresar todos los datos en los campos solicitados</t>
+  </si>
+  <si>
+    <t>Presionar el botón "registrarse"</t>
+  </si>
+  <si>
+    <t>En caso de que todos los campos sean validos se ingresará el usuario y recibirá automaticamente el rol de "vecino" y el estado de usuario "activo"</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Existen validación de datos, por lo que si el Rut, Correo o Telefono ingresado ya existe en la base de datos no podrá sobreescribirse, enviando una alerta al usuario que se está registrando. </t>
+  </si>
+  <si>
+    <t>Ingresar los datos de inicio de sesión</t>
+  </si>
+  <si>
+    <t>Correo y contraseña del usuario</t>
+  </si>
+  <si>
+    <t>En caso de que las credenciales sean válidas el usuario podrá iniciar sesión y será enviado a la página de inicio</t>
+  </si>
+  <si>
+    <t>Falta implementar las diferentes vistas que tienen los usuarios en base al rol (privilegios)</t>
+  </si>
+  <si>
+    <t>Ingresar los datos de inicio de sesión erróneos</t>
+  </si>
+  <si>
+    <t>Correo y contraseña del usuario no válidos</t>
+  </si>
+  <si>
+    <t>Si las credenciales no son válidas, se muestra una alerta de que el correo o la contraseña no son correctas</t>
+  </si>
+  <si>
+    <t>Seleccionar el rol del usuario para actualizar</t>
+  </si>
+  <si>
+    <t>El dropdown muestra los diferentes roles que existen</t>
+  </si>
+  <si>
+    <t>Dar click en el botón "actualizar"</t>
+  </si>
+  <si>
+    <t>El rol seleccionado será el nuevo rol del usuario</t>
+  </si>
+  <si>
+    <t>Se pueden implementar reglas de negocio para que no existan múltiples personas con el mismo rol, por ejemplo, con el rol de "presidente"</t>
+  </si>
+  <si>
+    <t>Seleccionar el estado del usuario para actualizar</t>
+  </si>
+  <si>
+    <t>El dropdown muestra los diferentes estados de usuario que existen (activo, inactivo y suspendido)</t>
+  </si>
+  <si>
+    <t>El estado seleccionado será el nuevo estado de usuario</t>
   </si>
 </sst>
 </file>
@@ -1390,11 +1471,8 @@
     <xf borderId="61" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="60" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="61" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf borderId="62" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="60" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
@@ -1479,6 +1557,9 @@
     <xf borderId="76" fillId="4" fontId="22" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="76" fillId="4" fontId="20" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="76" fillId="4" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="74" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -30316,9 +30397,15 @@
         <v>46</v>
       </c>
       <c r="C17" s="84"/>
-      <c r="D17" s="91"/>
-      <c r="E17" s="92"/>
-      <c r="F17" s="87"/>
+      <c r="D17" s="89" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="90" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" s="91" t="s">
+        <v>49</v>
+      </c>
       <c r="G17" s="88"/>
       <c r="H17" s="67"/>
       <c r="I17" s="1"/>
@@ -30343,12 +30430,18 @@
     <row r="18" ht="24.75" customHeight="1">
       <c r="A18" s="1"/>
       <c r="B18" s="83" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C18" s="84"/>
-      <c r="D18" s="91"/>
-      <c r="E18" s="92"/>
-      <c r="F18" s="87"/>
+      <c r="D18" s="89" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="90" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" s="91" t="s">
+        <v>49</v>
+      </c>
       <c r="G18" s="88"/>
       <c r="H18" s="67"/>
       <c r="I18" s="1"/>
@@ -30373,12 +30466,18 @@
     <row r="19" ht="24.75" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="83" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C19" s="84"/>
-      <c r="D19" s="91"/>
-      <c r="E19" s="92"/>
-      <c r="F19" s="87"/>
+      <c r="D19" s="89" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="90" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="91" t="s">
+        <v>49</v>
+      </c>
       <c r="G19" s="88"/>
       <c r="H19" s="67"/>
       <c r="I19" s="1"/>
@@ -30403,11 +30502,11 @@
     <row r="20" ht="24.75" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" s="83" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C20" s="84"/>
       <c r="D20" s="85"/>
-      <c r="E20" s="93"/>
+      <c r="E20" s="92"/>
       <c r="F20" s="87"/>
       <c r="G20" s="88"/>
       <c r="H20" s="67"/>
@@ -30433,11 +30532,11 @@
     <row r="21" ht="24.75" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="83" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="C21" s="84"/>
       <c r="D21" s="85"/>
-      <c r="E21" s="93"/>
+      <c r="E21" s="92"/>
       <c r="F21" s="87"/>
       <c r="G21" s="88"/>
       <c r="H21" s="67"/>
@@ -30463,11 +30562,11 @@
     <row r="22" ht="24.75" customHeight="1">
       <c r="A22" s="1"/>
       <c r="B22" s="83" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C22" s="84"/>
       <c r="D22" s="85"/>
-      <c r="E22" s="93"/>
+      <c r="E22" s="92"/>
       <c r="F22" s="87"/>
       <c r="G22" s="88"/>
       <c r="H22" s="67"/>
@@ -30492,12 +30591,12 @@
     </row>
     <row r="23" ht="19.5" customHeight="1">
       <c r="A23" s="1"/>
-      <c r="B23" s="94"/>
-      <c r="C23" s="95"/>
-      <c r="D23" s="95"/>
-      <c r="E23" s="95"/>
-      <c r="F23" s="95"/>
-      <c r="G23" s="95"/>
+      <c r="B23" s="93"/>
+      <c r="C23" s="94"/>
+      <c r="D23" s="94"/>
+      <c r="E23" s="94"/>
+      <c r="F23" s="94"/>
+      <c r="G23" s="94"/>
       <c r="H23" s="67"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -30520,12 +30619,12 @@
     </row>
     <row r="24" ht="19.5" customHeight="1">
       <c r="A24" s="2"/>
-      <c r="B24" s="96"/>
-      <c r="C24" s="96"/>
-      <c r="D24" s="96"/>
-      <c r="E24" s="96"/>
-      <c r="F24" s="95"/>
-      <c r="G24" s="95"/>
+      <c r="B24" s="95"/>
+      <c r="C24" s="95"/>
+      <c r="D24" s="95"/>
+      <c r="E24" s="95"/>
+      <c r="F24" s="94"/>
+      <c r="G24" s="94"/>
       <c r="H24" s="67"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -30548,12 +30647,12 @@
     </row>
     <row r="25" ht="19.5" customHeight="1">
       <c r="A25" s="1"/>
-      <c r="B25" s="97"/>
-      <c r="C25" s="98"/>
-      <c r="D25" s="96"/>
-      <c r="E25" s="96"/>
-      <c r="F25" s="96"/>
-      <c r="G25" s="96"/>
+      <c r="B25" s="96"/>
+      <c r="C25" s="97"/>
+      <c r="D25" s="95"/>
+      <c r="E25" s="95"/>
+      <c r="F25" s="95"/>
+      <c r="G25" s="95"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -30579,11 +30678,11 @@
       <c r="B26" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="99"/>
-      <c r="D26" s="100"/>
-      <c r="E26" s="101"/>
-      <c r="F26" s="101"/>
-      <c r="G26" s="101"/>
+      <c r="C26" s="98"/>
+      <c r="D26" s="99"/>
+      <c r="E26" s="100"/>
+      <c r="F26" s="100"/>
+      <c r="G26" s="100"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -30606,23 +30705,23 @@
     </row>
     <row r="27" ht="18.0" customHeight="1">
       <c r="A27" s="1"/>
-      <c r="B27" s="102" t="s">
-        <v>52</v>
+      <c r="B27" s="101" t="s">
+        <v>59</v>
       </c>
-      <c r="C27" s="103" t="s">
-        <v>53</v>
+      <c r="C27" s="102" t="s">
+        <v>60</v>
       </c>
-      <c r="D27" s="103" t="s">
-        <v>54</v>
+      <c r="D27" s="102" t="s">
+        <v>61</v>
       </c>
-      <c r="E27" s="103" t="s">
-        <v>55</v>
+      <c r="E27" s="102" t="s">
+        <v>62</v>
       </c>
-      <c r="F27" s="104" t="s">
-        <v>56</v>
+      <c r="F27" s="103" t="s">
+        <v>63</v>
       </c>
-      <c r="G27" s="105" t="s">
-        <v>57</v>
+      <c r="G27" s="104" t="s">
+        <v>64</v>
       </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
@@ -30646,20 +30745,20 @@
     </row>
     <row r="28" ht="34.5" customHeight="1">
       <c r="A28" s="1"/>
-      <c r="B28" s="106">
+      <c r="B28" s="105">
         <v>1.0</v>
       </c>
-      <c r="C28" s="107" t="s">
-        <v>58</v>
+      <c r="C28" s="106" t="s">
+        <v>65</v>
       </c>
-      <c r="D28" s="108"/>
-      <c r="E28" s="109" t="s">
-        <v>59</v>
+      <c r="D28" s="107"/>
+      <c r="E28" s="108" t="s">
+        <v>66</v>
       </c>
-      <c r="F28" s="110" t="s">
-        <v>60</v>
+      <c r="F28" s="109" t="s">
+        <v>67</v>
       </c>
-      <c r="G28" s="111"/>
+      <c r="G28" s="110"/>
       <c r="H28" s="67"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
@@ -30682,21 +30781,21 @@
     </row>
     <row r="29" ht="34.5" customHeight="1">
       <c r="A29" s="1"/>
-      <c r="B29" s="106">
+      <c r="B29" s="105">
         <v>2.0</v>
       </c>
-      <c r="C29" s="107" t="s">
-        <v>61</v>
+      <c r="C29" s="106" t="s">
+        <v>68</v>
       </c>
-      <c r="D29" s="108"/>
-      <c r="E29" s="109" t="s">
-        <v>62</v>
+      <c r="D29" s="107"/>
+      <c r="E29" s="108" t="s">
+        <v>69</v>
       </c>
-      <c r="F29" s="110" t="s">
-        <v>60</v>
+      <c r="F29" s="109" t="s">
+        <v>67</v>
       </c>
-      <c r="G29" s="110" t="s">
-        <v>63</v>
+      <c r="G29" s="109" t="s">
+        <v>70</v>
       </c>
       <c r="H29" s="67"/>
       <c r="I29" s="1"/>
@@ -30720,18 +30819,18 @@
     </row>
     <row r="30" ht="34.5" customHeight="1">
       <c r="A30" s="1"/>
-      <c r="B30" s="106">
+      <c r="B30" s="105">
         <v>3.0</v>
       </c>
-      <c r="C30" s="112" t="s">
-        <v>64</v>
+      <c r="C30" s="111" t="s">
+        <v>71</v>
       </c>
-      <c r="D30" s="108"/>
-      <c r="E30" s="113" t="s">
-        <v>65</v>
+      <c r="D30" s="107"/>
+      <c r="E30" s="112" t="s">
+        <v>72</v>
       </c>
-      <c r="F30" s="111"/>
-      <c r="G30" s="111"/>
+      <c r="F30" s="110"/>
+      <c r="G30" s="110"/>
       <c r="H30" s="67"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
@@ -30754,14 +30853,14 @@
     </row>
     <row r="31" ht="34.5" customHeight="1">
       <c r="A31" s="1"/>
-      <c r="B31" s="106">
+      <c r="B31" s="105">
         <v>4.0</v>
       </c>
-      <c r="C31" s="107"/>
-      <c r="D31" s="108"/>
-      <c r="E31" s="109"/>
-      <c r="F31" s="111"/>
-      <c r="G31" s="111"/>
+      <c r="C31" s="106"/>
+      <c r="D31" s="107"/>
+      <c r="E31" s="108"/>
+      <c r="F31" s="110"/>
+      <c r="G31" s="110"/>
       <c r="H31" s="67"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
@@ -30784,14 +30883,14 @@
     </row>
     <row r="32" ht="34.5" customHeight="1">
       <c r="A32" s="1"/>
-      <c r="B32" s="106">
+      <c r="B32" s="105">
         <v>5.0</v>
       </c>
-      <c r="C32" s="107"/>
-      <c r="D32" s="108"/>
-      <c r="E32" s="109"/>
-      <c r="F32" s="111"/>
-      <c r="G32" s="111"/>
+      <c r="C32" s="106"/>
+      <c r="D32" s="107"/>
+      <c r="E32" s="108"/>
+      <c r="F32" s="110"/>
+      <c r="G32" s="110"/>
       <c r="H32" s="67"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
@@ -30814,14 +30913,14 @@
     </row>
     <row r="33" ht="34.5" customHeight="1">
       <c r="A33" s="1"/>
-      <c r="B33" s="114">
+      <c r="B33" s="113">
         <v>6.0</v>
       </c>
-      <c r="C33" s="107"/>
-      <c r="D33" s="115"/>
-      <c r="E33" s="109"/>
-      <c r="F33" s="111"/>
-      <c r="G33" s="111"/>
+      <c r="C33" s="106"/>
+      <c r="D33" s="114"/>
+      <c r="E33" s="108"/>
+      <c r="F33" s="110"/>
+      <c r="G33" s="110"/>
       <c r="H33" s="67"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
@@ -30844,12 +30943,12 @@
     </row>
     <row r="34" ht="19.5" customHeight="1">
       <c r="A34" s="1"/>
-      <c r="B34" s="116"/>
-      <c r="C34" s="116"/>
+      <c r="B34" s="115"/>
+      <c r="C34" s="115"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
-      <c r="F34" s="117"/>
-      <c r="G34" s="117"/>
+      <c r="F34" s="116"/>
+      <c r="G34" s="116"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
@@ -30872,14 +30971,14 @@
     </row>
     <row r="35" ht="19.5" customHeight="1">
       <c r="A35" s="1"/>
-      <c r="B35" s="118" t="s">
+      <c r="B35" s="117" t="s">
         <v>37</v>
       </c>
-      <c r="C35" s="99"/>
-      <c r="D35" s="100"/>
-      <c r="E35" s="101"/>
-      <c r="F35" s="101"/>
-      <c r="G35" s="101"/>
+      <c r="C35" s="98"/>
+      <c r="D35" s="99"/>
+      <c r="E35" s="100"/>
+      <c r="F35" s="100"/>
+      <c r="G35" s="100"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
@@ -30902,23 +31001,23 @@
     </row>
     <row r="36" ht="18.0" customHeight="1">
       <c r="A36" s="1"/>
-      <c r="B36" s="102" t="s">
-        <v>52</v>
+      <c r="B36" s="101" t="s">
+        <v>59</v>
       </c>
-      <c r="C36" s="103" t="s">
-        <v>53</v>
+      <c r="C36" s="102" t="s">
+        <v>60</v>
       </c>
-      <c r="D36" s="103" t="s">
-        <v>54</v>
+      <c r="D36" s="102" t="s">
+        <v>61</v>
       </c>
-      <c r="E36" s="103" t="s">
-        <v>55</v>
+      <c r="E36" s="102" t="s">
+        <v>62</v>
       </c>
-      <c r="F36" s="104" t="s">
-        <v>56</v>
+      <c r="F36" s="103" t="s">
+        <v>63</v>
       </c>
-      <c r="G36" s="105" t="s">
-        <v>57</v>
+      <c r="G36" s="104" t="s">
+        <v>64</v>
       </c>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
@@ -30942,20 +31041,20 @@
     </row>
     <row r="37" ht="34.5" customHeight="1">
       <c r="A37" s="1"/>
-      <c r="B37" s="106">
+      <c r="B37" s="105">
         <v>1.0</v>
       </c>
-      <c r="C37" s="107" t="s">
-        <v>58</v>
+      <c r="C37" s="106" t="s">
+        <v>65</v>
       </c>
-      <c r="D37" s="108"/>
-      <c r="E37" s="109" t="s">
-        <v>59</v>
+      <c r="D37" s="107"/>
+      <c r="E37" s="108" t="s">
+        <v>66</v>
       </c>
-      <c r="F37" s="110" t="s">
-        <v>60</v>
+      <c r="F37" s="109" t="s">
+        <v>67</v>
       </c>
-      <c r="G37" s="111"/>
+      <c r="G37" s="110"/>
       <c r="H37" s="67"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
@@ -30978,21 +31077,21 @@
     </row>
     <row r="38" ht="34.5" customHeight="1">
       <c r="A38" s="1"/>
-      <c r="B38" s="106">
+      <c r="B38" s="105">
         <v>2.0</v>
       </c>
-      <c r="C38" s="107" t="s">
-        <v>61</v>
+      <c r="C38" s="106" t="s">
+        <v>68</v>
       </c>
-      <c r="D38" s="108"/>
-      <c r="E38" s="109" t="s">
-        <v>62</v>
+      <c r="D38" s="107"/>
+      <c r="E38" s="108" t="s">
+        <v>69</v>
       </c>
-      <c r="F38" s="110" t="s">
-        <v>60</v>
+      <c r="F38" s="109" t="s">
+        <v>67</v>
       </c>
-      <c r="G38" s="110" t="s">
-        <v>63</v>
+      <c r="G38" s="109" t="s">
+        <v>70</v>
       </c>
       <c r="H38" s="67"/>
       <c r="J38" s="1"/>
@@ -31015,18 +31114,18 @@
     </row>
     <row r="39" ht="34.5" customHeight="1">
       <c r="A39" s="1"/>
-      <c r="B39" s="106">
+      <c r="B39" s="105">
         <v>3.0</v>
       </c>
-      <c r="C39" s="112" t="s">
-        <v>64</v>
+      <c r="C39" s="111" t="s">
+        <v>71</v>
       </c>
-      <c r="D39" s="108"/>
-      <c r="E39" s="113" t="s">
-        <v>65</v>
+      <c r="D39" s="107"/>
+      <c r="E39" s="112" t="s">
+        <v>72</v>
       </c>
-      <c r="F39" s="111"/>
-      <c r="G39" s="111"/>
+      <c r="F39" s="110"/>
+      <c r="G39" s="110"/>
       <c r="H39" s="67"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
@@ -31049,14 +31148,14 @@
     </row>
     <row r="40" ht="34.5" customHeight="1">
       <c r="A40" s="1"/>
-      <c r="B40" s="106">
+      <c r="B40" s="105">
         <v>4.0</v>
       </c>
-      <c r="C40" s="119"/>
-      <c r="D40" s="108"/>
-      <c r="E40" s="109"/>
-      <c r="F40" s="111"/>
-      <c r="G40" s="111"/>
+      <c r="C40" s="118"/>
+      <c r="D40" s="107"/>
+      <c r="E40" s="108"/>
+      <c r="F40" s="110"/>
+      <c r="G40" s="110"/>
       <c r="H40" s="67"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
@@ -31079,14 +31178,14 @@
     </row>
     <row r="41" ht="34.5" customHeight="1">
       <c r="A41" s="1"/>
-      <c r="B41" s="106">
+      <c r="B41" s="105">
         <v>5.0</v>
       </c>
-      <c r="C41" s="107"/>
-      <c r="D41" s="108"/>
-      <c r="E41" s="109"/>
-      <c r="F41" s="111"/>
-      <c r="G41" s="111"/>
+      <c r="C41" s="106"/>
+      <c r="D41" s="107"/>
+      <c r="E41" s="108"/>
+      <c r="F41" s="110"/>
+      <c r="G41" s="110"/>
       <c r="H41" s="67"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
@@ -31109,14 +31208,14 @@
     </row>
     <row r="42" ht="34.5" customHeight="1">
       <c r="A42" s="1"/>
-      <c r="B42" s="114">
+      <c r="B42" s="113">
         <v>6.0</v>
       </c>
-      <c r="C42" s="107"/>
-      <c r="D42" s="115"/>
-      <c r="E42" s="109"/>
-      <c r="F42" s="111"/>
-      <c r="G42" s="111"/>
+      <c r="C42" s="106"/>
+      <c r="D42" s="114"/>
+      <c r="E42" s="108"/>
+      <c r="F42" s="110"/>
+      <c r="G42" s="110"/>
       <c r="H42" s="67"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
@@ -31139,12 +31238,12 @@
     </row>
     <row r="43" ht="19.5" customHeight="1">
       <c r="A43" s="2"/>
-      <c r="B43" s="120"/>
-      <c r="C43" s="121"/>
-      <c r="D43" s="121"/>
-      <c r="E43" s="121"/>
-      <c r="F43" s="122"/>
-      <c r="G43" s="122"/>
+      <c r="B43" s="119"/>
+      <c r="C43" s="120"/>
+      <c r="D43" s="120"/>
+      <c r="E43" s="120"/>
+      <c r="F43" s="121"/>
+      <c r="G43" s="121"/>
       <c r="H43" s="67"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
@@ -31167,14 +31266,14 @@
     </row>
     <row r="44" ht="19.5" customHeight="1">
       <c r="A44" s="1"/>
-      <c r="B44" s="118" t="s">
+      <c r="B44" s="117" t="s">
         <v>40</v>
       </c>
-      <c r="C44" s="99"/>
-      <c r="D44" s="100"/>
-      <c r="E44" s="101"/>
-      <c r="F44" s="101"/>
-      <c r="G44" s="101"/>
+      <c r="C44" s="98"/>
+      <c r="D44" s="99"/>
+      <c r="E44" s="100"/>
+      <c r="F44" s="100"/>
+      <c r="G44" s="100"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
@@ -31197,23 +31296,23 @@
     </row>
     <row r="45" ht="18.0" customHeight="1">
       <c r="A45" s="1"/>
-      <c r="B45" s="102" t="s">
-        <v>52</v>
+      <c r="B45" s="101" t="s">
+        <v>59</v>
       </c>
-      <c r="C45" s="103" t="s">
-        <v>53</v>
+      <c r="C45" s="102" t="s">
+        <v>60</v>
       </c>
-      <c r="D45" s="103" t="s">
-        <v>54</v>
+      <c r="D45" s="102" t="s">
+        <v>61</v>
       </c>
-      <c r="E45" s="103" t="s">
-        <v>55</v>
+      <c r="E45" s="102" t="s">
+        <v>62</v>
       </c>
-      <c r="F45" s="104" t="s">
-        <v>56</v>
+      <c r="F45" s="103" t="s">
+        <v>63</v>
       </c>
-      <c r="G45" s="105" t="s">
-        <v>57</v>
+      <c r="G45" s="104" t="s">
+        <v>64</v>
       </c>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
@@ -31237,20 +31336,20 @@
     </row>
     <row r="46" ht="34.5" customHeight="1">
       <c r="A46" s="1"/>
-      <c r="B46" s="106">
+      <c r="B46" s="105">
         <v>1.0</v>
       </c>
-      <c r="C46" s="107" t="s">
-        <v>58</v>
+      <c r="C46" s="106" t="s">
+        <v>65</v>
       </c>
-      <c r="D46" s="108"/>
-      <c r="E46" s="109" t="s">
-        <v>59</v>
+      <c r="D46" s="107"/>
+      <c r="E46" s="108" t="s">
+        <v>66</v>
       </c>
-      <c r="F46" s="110" t="s">
-        <v>60</v>
+      <c r="F46" s="109" t="s">
+        <v>67</v>
       </c>
-      <c r="G46" s="111"/>
+      <c r="G46" s="110"/>
       <c r="H46" s="67"/>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
@@ -31273,21 +31372,21 @@
     </row>
     <row r="47" ht="34.5" customHeight="1">
       <c r="A47" s="1"/>
-      <c r="B47" s="106">
+      <c r="B47" s="105">
         <v>2.0</v>
       </c>
-      <c r="C47" s="107" t="s">
-        <v>61</v>
+      <c r="C47" s="106" t="s">
+        <v>68</v>
       </c>
-      <c r="D47" s="108"/>
-      <c r="E47" s="109" t="s">
-        <v>62</v>
+      <c r="D47" s="107"/>
+      <c r="E47" s="108" t="s">
+        <v>69</v>
       </c>
-      <c r="F47" s="110" t="s">
-        <v>60</v>
+      <c r="F47" s="109" t="s">
+        <v>67</v>
       </c>
-      <c r="G47" s="110" t="s">
-        <v>63</v>
+      <c r="G47" s="109" t="s">
+        <v>70</v>
       </c>
       <c r="H47" s="67"/>
       <c r="I47" s="1"/>
@@ -31311,18 +31410,18 @@
     </row>
     <row r="48" ht="34.5" customHeight="1">
       <c r="A48" s="1"/>
-      <c r="B48" s="106">
+      <c r="B48" s="105">
         <v>3.0</v>
       </c>
-      <c r="C48" s="112" t="s">
-        <v>64</v>
+      <c r="C48" s="111" t="s">
+        <v>71</v>
       </c>
-      <c r="D48" s="108"/>
-      <c r="E48" s="113" t="s">
-        <v>65</v>
+      <c r="D48" s="107"/>
+      <c r="E48" s="112" t="s">
+        <v>72</v>
       </c>
-      <c r="F48" s="111"/>
-      <c r="G48" s="111"/>
+      <c r="F48" s="110"/>
+      <c r="G48" s="110"/>
       <c r="H48" s="67"/>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
@@ -31345,14 +31444,14 @@
     </row>
     <row r="49" ht="34.5" customHeight="1">
       <c r="A49" s="1"/>
-      <c r="B49" s="106">
+      <c r="B49" s="105">
         <v>4.0</v>
       </c>
-      <c r="C49" s="119"/>
-      <c r="D49" s="108"/>
-      <c r="E49" s="109"/>
-      <c r="F49" s="111"/>
-      <c r="G49" s="111"/>
+      <c r="C49" s="118"/>
+      <c r="D49" s="107"/>
+      <c r="E49" s="108"/>
+      <c r="F49" s="110"/>
+      <c r="G49" s="110"/>
       <c r="H49" s="67"/>
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
@@ -31375,14 +31474,14 @@
     </row>
     <row r="50" ht="34.5" customHeight="1">
       <c r="A50" s="1"/>
-      <c r="B50" s="106">
+      <c r="B50" s="105">
         <v>5.0</v>
       </c>
-      <c r="C50" s="107"/>
-      <c r="D50" s="108"/>
-      <c r="E50" s="109"/>
-      <c r="F50" s="111"/>
-      <c r="G50" s="111"/>
+      <c r="C50" s="106"/>
+      <c r="D50" s="107"/>
+      <c r="E50" s="108"/>
+      <c r="F50" s="110"/>
+      <c r="G50" s="110"/>
       <c r="H50" s="67"/>
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
@@ -31405,14 +31504,14 @@
     </row>
     <row r="51" ht="34.5" customHeight="1">
       <c r="A51" s="1"/>
-      <c r="B51" s="114">
+      <c r="B51" s="113">
         <v>6.0</v>
       </c>
-      <c r="C51" s="107"/>
-      <c r="D51" s="115"/>
-      <c r="E51" s="109"/>
-      <c r="F51" s="111"/>
-      <c r="G51" s="111"/>
+      <c r="C51" s="106"/>
+      <c r="D51" s="114"/>
+      <c r="E51" s="108"/>
+      <c r="F51" s="110"/>
+      <c r="G51" s="110"/>
       <c r="H51" s="67"/>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
@@ -31435,8 +31534,8 @@
     </row>
     <row r="52" ht="19.5" customHeight="1">
       <c r="A52" s="2"/>
-      <c r="B52" s="123"/>
-      <c r="C52" s="124"/>
+      <c r="B52" s="122"/>
+      <c r="C52" s="123"/>
       <c r="D52" s="57"/>
       <c r="E52" s="57"/>
       <c r="F52" s="1"/>
@@ -31463,14 +31562,14 @@
     </row>
     <row r="53" ht="19.5" customHeight="1">
       <c r="A53" s="1"/>
-      <c r="B53" s="118" t="s">
+      <c r="B53" s="117" t="s">
         <v>43</v>
       </c>
-      <c r="C53" s="99"/>
-      <c r="D53" s="100"/>
-      <c r="E53" s="101"/>
-      <c r="F53" s="101"/>
-      <c r="G53" s="101"/>
+      <c r="C53" s="98"/>
+      <c r="D53" s="99"/>
+      <c r="E53" s="100"/>
+      <c r="F53" s="100"/>
+      <c r="G53" s="100"/>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
@@ -31493,23 +31592,23 @@
     </row>
     <row r="54" ht="18.0" customHeight="1">
       <c r="A54" s="1"/>
-      <c r="B54" s="102" t="s">
-        <v>52</v>
+      <c r="B54" s="101" t="s">
+        <v>59</v>
       </c>
-      <c r="C54" s="103" t="s">
-        <v>53</v>
+      <c r="C54" s="102" t="s">
+        <v>60</v>
       </c>
-      <c r="D54" s="103" t="s">
-        <v>54</v>
+      <c r="D54" s="102" t="s">
+        <v>61</v>
       </c>
-      <c r="E54" s="103" t="s">
-        <v>55</v>
+      <c r="E54" s="102" t="s">
+        <v>62</v>
       </c>
-      <c r="F54" s="104" t="s">
-        <v>56</v>
+      <c r="F54" s="103" t="s">
+        <v>63</v>
       </c>
-      <c r="G54" s="105" t="s">
-        <v>57</v>
+      <c r="G54" s="104" t="s">
+        <v>64</v>
       </c>
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
@@ -31533,20 +31632,20 @@
     </row>
     <row r="55" ht="34.5" customHeight="1">
       <c r="A55" s="1"/>
-      <c r="B55" s="106">
+      <c r="B55" s="105">
         <v>1.0</v>
       </c>
-      <c r="C55" s="107" t="s">
-        <v>58</v>
+      <c r="C55" s="106" t="s">
+        <v>65</v>
       </c>
-      <c r="D55" s="108"/>
-      <c r="E55" s="109" t="s">
-        <v>59</v>
+      <c r="D55" s="107"/>
+      <c r="E55" s="108" t="s">
+        <v>66</v>
       </c>
-      <c r="F55" s="110" t="s">
-        <v>60</v>
+      <c r="F55" s="109" t="s">
+        <v>67</v>
       </c>
-      <c r="G55" s="111"/>
+      <c r="G55" s="110"/>
       <c r="H55" s="67"/>
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
@@ -31569,21 +31668,21 @@
     </row>
     <row r="56" ht="34.5" customHeight="1">
       <c r="A56" s="1"/>
-      <c r="B56" s="106">
+      <c r="B56" s="105">
         <v>2.0</v>
       </c>
-      <c r="C56" s="107" t="s">
-        <v>61</v>
+      <c r="C56" s="106" t="s">
+        <v>68</v>
       </c>
-      <c r="D56" s="108"/>
-      <c r="E56" s="109" t="s">
-        <v>62</v>
+      <c r="D56" s="107"/>
+      <c r="E56" s="108" t="s">
+        <v>69</v>
       </c>
-      <c r="F56" s="110" t="s">
-        <v>60</v>
+      <c r="F56" s="109" t="s">
+        <v>67</v>
       </c>
-      <c r="G56" s="110" t="s">
-        <v>63</v>
+      <c r="G56" s="109" t="s">
+        <v>70</v>
       </c>
       <c r="H56" s="67"/>
       <c r="I56" s="1"/>
@@ -31607,18 +31706,18 @@
     </row>
     <row r="57" ht="34.5" customHeight="1">
       <c r="A57" s="1"/>
-      <c r="B57" s="106">
+      <c r="B57" s="105">
         <v>3.0</v>
       </c>
-      <c r="C57" s="112" t="s">
-        <v>64</v>
+      <c r="C57" s="111" t="s">
+        <v>71</v>
       </c>
-      <c r="D57" s="108"/>
-      <c r="E57" s="113" t="s">
-        <v>65</v>
+      <c r="D57" s="107"/>
+      <c r="E57" s="112" t="s">
+        <v>72</v>
       </c>
-      <c r="F57" s="111"/>
-      <c r="G57" s="111"/>
+      <c r="F57" s="110"/>
+      <c r="G57" s="110"/>
       <c r="H57" s="67"/>
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
@@ -31641,14 +31740,14 @@
     </row>
     <row r="58" ht="34.5" customHeight="1">
       <c r="A58" s="1"/>
-      <c r="B58" s="106">
+      <c r="B58" s="105">
         <v>4.0</v>
       </c>
-      <c r="C58" s="119"/>
-      <c r="D58" s="108"/>
-      <c r="E58" s="109"/>
-      <c r="F58" s="111"/>
-      <c r="G58" s="111"/>
+      <c r="C58" s="118"/>
+      <c r="D58" s="107"/>
+      <c r="E58" s="108"/>
+      <c r="F58" s="110"/>
+      <c r="G58" s="110"/>
       <c r="H58" s="67"/>
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
@@ -31671,14 +31770,14 @@
     </row>
     <row r="59" ht="34.5" customHeight="1">
       <c r="A59" s="1"/>
-      <c r="B59" s="106">
+      <c r="B59" s="105">
         <v>5.0</v>
       </c>
-      <c r="C59" s="107"/>
-      <c r="D59" s="108"/>
-      <c r="E59" s="109"/>
-      <c r="F59" s="111"/>
-      <c r="G59" s="111"/>
+      <c r="C59" s="106"/>
+      <c r="D59" s="107"/>
+      <c r="E59" s="108"/>
+      <c r="F59" s="110"/>
+      <c r="G59" s="110"/>
       <c r="H59" s="67"/>
       <c r="I59" s="1"/>
       <c r="J59" s="1"/>
@@ -31701,14 +31800,14 @@
     </row>
     <row r="60" ht="34.5" customHeight="1">
       <c r="A60" s="1"/>
-      <c r="B60" s="114">
+      <c r="B60" s="113">
         <v>6.0</v>
       </c>
-      <c r="C60" s="107"/>
-      <c r="D60" s="115"/>
-      <c r="E60" s="109"/>
-      <c r="F60" s="111"/>
-      <c r="G60" s="111"/>
+      <c r="C60" s="106"/>
+      <c r="D60" s="114"/>
+      <c r="E60" s="108"/>
+      <c r="F60" s="110"/>
+      <c r="G60" s="110"/>
       <c r="H60" s="67"/>
       <c r="I60" s="1"/>
       <c r="J60" s="1"/>
@@ -31731,8 +31830,8 @@
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="1"/>
-      <c r="B61" s="125"/>
-      <c r="C61" s="125"/>
+      <c r="B61" s="124"/>
+      <c r="C61" s="124"/>
       <c r="D61" s="57"/>
       <c r="E61" s="57"/>
       <c r="F61" s="1"/>
@@ -31759,14 +31858,14 @@
     </row>
     <row r="62" ht="15.75" customHeight="1">
       <c r="A62" s="1"/>
-      <c r="B62" s="118" t="s">
+      <c r="B62" s="117" t="s">
         <v>46</v>
       </c>
-      <c r="C62" s="99"/>
-      <c r="D62" s="100"/>
-      <c r="E62" s="101"/>
-      <c r="F62" s="101"/>
-      <c r="G62" s="101"/>
+      <c r="C62" s="98"/>
+      <c r="D62" s="99"/>
+      <c r="E62" s="100"/>
+      <c r="F62" s="100"/>
+      <c r="G62" s="100"/>
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
@@ -31789,23 +31888,23 @@
     </row>
     <row r="63" ht="18.0" customHeight="1">
       <c r="A63" s="1"/>
-      <c r="B63" s="102" t="s">
-        <v>52</v>
+      <c r="B63" s="101" t="s">
+        <v>59</v>
       </c>
-      <c r="C63" s="103" t="s">
-        <v>53</v>
+      <c r="C63" s="102" t="s">
+        <v>60</v>
       </c>
-      <c r="D63" s="103" t="s">
-        <v>54</v>
+      <c r="D63" s="102" t="s">
+        <v>61</v>
       </c>
-      <c r="E63" s="103" t="s">
-        <v>55</v>
+      <c r="E63" s="102" t="s">
+        <v>62</v>
       </c>
-      <c r="F63" s="104" t="s">
-        <v>56</v>
+      <c r="F63" s="103" t="s">
+        <v>63</v>
       </c>
-      <c r="G63" s="105" t="s">
-        <v>57</v>
+      <c r="G63" s="104" t="s">
+        <v>64</v>
       </c>
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
@@ -31829,14 +31928,16 @@
     </row>
     <row r="64" ht="34.5" customHeight="1">
       <c r="A64" s="1"/>
-      <c r="B64" s="106">
+      <c r="B64" s="105">
         <v>1.0</v>
       </c>
-      <c r="C64" s="107"/>
-      <c r="D64" s="108"/>
-      <c r="E64" s="109"/>
-      <c r="F64" s="111"/>
-      <c r="G64" s="111"/>
+      <c r="C64" s="111" t="s">
+        <v>73</v>
+      </c>
+      <c r="D64" s="107"/>
+      <c r="E64" s="112"/>
+      <c r="F64" s="109"/>
+      <c r="G64" s="110"/>
       <c r="H64" s="67"/>
       <c r="I64" s="1"/>
       <c r="J64" s="1"/>
@@ -31859,14 +31960,22 @@
     </row>
     <row r="65" ht="34.5" customHeight="1">
       <c r="A65" s="1"/>
-      <c r="B65" s="106">
+      <c r="B65" s="105">
         <v>2.0</v>
       </c>
-      <c r="C65" s="107"/>
-      <c r="D65" s="108"/>
-      <c r="E65" s="109"/>
-      <c r="F65" s="111"/>
-      <c r="G65" s="111"/>
+      <c r="C65" s="111" t="s">
+        <v>74</v>
+      </c>
+      <c r="D65" s="107"/>
+      <c r="E65" s="112" t="s">
+        <v>75</v>
+      </c>
+      <c r="F65" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="G65" s="109" t="s">
+        <v>77</v>
+      </c>
       <c r="H65" s="67"/>
       <c r="I65" s="1"/>
       <c r="J65" s="1"/>
@@ -31889,14 +31998,14 @@
     </row>
     <row r="66" ht="34.5" customHeight="1">
       <c r="A66" s="1"/>
-      <c r="B66" s="106">
+      <c r="B66" s="105">
         <v>3.0</v>
       </c>
-      <c r="C66" s="107"/>
-      <c r="D66" s="108"/>
-      <c r="E66" s="109"/>
-      <c r="F66" s="111"/>
-      <c r="G66" s="111"/>
+      <c r="C66" s="106"/>
+      <c r="D66" s="107"/>
+      <c r="E66" s="108"/>
+      <c r="F66" s="110"/>
+      <c r="G66" s="110"/>
       <c r="H66" s="67"/>
       <c r="I66" s="1"/>
       <c r="J66" s="1"/>
@@ -31919,14 +32028,14 @@
     </row>
     <row r="67" ht="34.5" customHeight="1">
       <c r="A67" s="1"/>
-      <c r="B67" s="106">
+      <c r="B67" s="105">
         <v>4.0</v>
       </c>
-      <c r="C67" s="119"/>
-      <c r="D67" s="108"/>
-      <c r="E67" s="109"/>
-      <c r="F67" s="111"/>
-      <c r="G67" s="111"/>
+      <c r="C67" s="118"/>
+      <c r="D67" s="107"/>
+      <c r="E67" s="108"/>
+      <c r="F67" s="110"/>
+      <c r="G67" s="110"/>
       <c r="H67" s="67"/>
       <c r="I67" s="1"/>
       <c r="J67" s="1"/>
@@ -31949,14 +32058,14 @@
     </row>
     <row r="68" ht="34.5" customHeight="1">
       <c r="A68" s="1"/>
-      <c r="B68" s="106">
+      <c r="B68" s="105">
         <v>5.0</v>
       </c>
-      <c r="C68" s="107"/>
-      <c r="D68" s="108"/>
-      <c r="E68" s="109"/>
-      <c r="F68" s="111"/>
-      <c r="G68" s="111"/>
+      <c r="C68" s="106"/>
+      <c r="D68" s="107"/>
+      <c r="E68" s="108"/>
+      <c r="F68" s="110"/>
+      <c r="G68" s="110"/>
       <c r="H68" s="67"/>
       <c r="I68" s="1"/>
       <c r="J68" s="1"/>
@@ -31979,14 +32088,14 @@
     </row>
     <row r="69" ht="34.5" customHeight="1">
       <c r="A69" s="1"/>
-      <c r="B69" s="114">
+      <c r="B69" s="113">
         <v>6.0</v>
       </c>
-      <c r="C69" s="107"/>
-      <c r="D69" s="115"/>
-      <c r="E69" s="109"/>
-      <c r="F69" s="111"/>
-      <c r="G69" s="111"/>
+      <c r="C69" s="106"/>
+      <c r="D69" s="114"/>
+      <c r="E69" s="108"/>
+      <c r="F69" s="110"/>
+      <c r="G69" s="110"/>
       <c r="H69" s="67"/>
       <c r="I69" s="1"/>
       <c r="J69" s="1"/>
@@ -32009,8 +32118,8 @@
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" s="1"/>
-      <c r="B70" s="116"/>
-      <c r="C70" s="116"/>
+      <c r="B70" s="115"/>
+      <c r="C70" s="115"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
@@ -32037,14 +32146,14 @@
     </row>
     <row r="71" ht="15.75" customHeight="1">
       <c r="A71" s="1"/>
-      <c r="B71" s="118" t="s">
-        <v>47</v>
+      <c r="B71" s="117" t="s">
+        <v>50</v>
       </c>
-      <c r="C71" s="99"/>
-      <c r="D71" s="100"/>
-      <c r="E71" s="101"/>
-      <c r="F71" s="101"/>
-      <c r="G71" s="101"/>
+      <c r="C71" s="98"/>
+      <c r="D71" s="99"/>
+      <c r="E71" s="100"/>
+      <c r="F71" s="100"/>
+      <c r="G71" s="100"/>
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
       <c r="J71" s="1"/>
@@ -32067,23 +32176,23 @@
     </row>
     <row r="72" ht="18.0" customHeight="1">
       <c r="A72" s="1"/>
-      <c r="B72" s="102" t="s">
-        <v>52</v>
+      <c r="B72" s="101" t="s">
+        <v>59</v>
       </c>
-      <c r="C72" s="103" t="s">
-        <v>53</v>
+      <c r="C72" s="102" t="s">
+        <v>60</v>
       </c>
-      <c r="D72" s="103" t="s">
-        <v>54</v>
+      <c r="D72" s="102" t="s">
+        <v>61</v>
       </c>
-      <c r="E72" s="103" t="s">
-        <v>55</v>
+      <c r="E72" s="102" t="s">
+        <v>62</v>
       </c>
-      <c r="F72" s="104" t="s">
-        <v>56</v>
+      <c r="F72" s="103" t="s">
+        <v>63</v>
       </c>
-      <c r="G72" s="105" t="s">
-        <v>57</v>
+      <c r="G72" s="104" t="s">
+        <v>64</v>
       </c>
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
@@ -32107,14 +32216,24 @@
     </row>
     <row r="73" ht="34.5" customHeight="1">
       <c r="A73" s="1"/>
-      <c r="B73" s="106">
+      <c r="B73" s="105">
         <v>1.0</v>
       </c>
-      <c r="C73" s="107"/>
-      <c r="D73" s="108"/>
-      <c r="E73" s="109"/>
-      <c r="F73" s="111"/>
-      <c r="G73" s="111"/>
+      <c r="C73" s="111" t="s">
+        <v>78</v>
+      </c>
+      <c r="D73" s="125" t="s">
+        <v>79</v>
+      </c>
+      <c r="E73" s="112" t="s">
+        <v>80</v>
+      </c>
+      <c r="F73" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="G73" s="109" t="s">
+        <v>81</v>
+      </c>
       <c r="H73" s="67"/>
       <c r="I73" s="1"/>
       <c r="J73" s="1"/>
@@ -32137,14 +32256,22 @@
     </row>
     <row r="74" ht="34.5" customHeight="1">
       <c r="A74" s="1"/>
-      <c r="B74" s="106">
+      <c r="B74" s="105">
         <v>2.0</v>
       </c>
-      <c r="C74" s="107"/>
-      <c r="D74" s="108"/>
-      <c r="E74" s="109"/>
-      <c r="F74" s="111"/>
-      <c r="G74" s="111"/>
+      <c r="C74" s="111" t="s">
+        <v>82</v>
+      </c>
+      <c r="D74" s="125" t="s">
+        <v>83</v>
+      </c>
+      <c r="E74" s="112" t="s">
+        <v>84</v>
+      </c>
+      <c r="F74" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="G74" s="110"/>
       <c r="H74" s="67"/>
       <c r="I74" s="1"/>
       <c r="J74" s="1"/>
@@ -32167,14 +32294,14 @@
     </row>
     <row r="75" ht="34.5" customHeight="1">
       <c r="A75" s="1"/>
-      <c r="B75" s="106">
+      <c r="B75" s="105">
         <v>3.0</v>
       </c>
-      <c r="C75" s="107"/>
-      <c r="D75" s="108"/>
-      <c r="E75" s="109"/>
-      <c r="F75" s="111"/>
-      <c r="G75" s="111"/>
+      <c r="C75" s="106"/>
+      <c r="D75" s="107"/>
+      <c r="E75" s="108"/>
+      <c r="F75" s="110"/>
+      <c r="G75" s="110"/>
       <c r="H75" s="67"/>
       <c r="I75" s="1"/>
       <c r="J75" s="1"/>
@@ -32197,14 +32324,14 @@
     </row>
     <row r="76" ht="34.5" customHeight="1">
       <c r="A76" s="1"/>
-      <c r="B76" s="106">
+      <c r="B76" s="105">
         <v>4.0</v>
       </c>
-      <c r="C76" s="119"/>
-      <c r="D76" s="108"/>
-      <c r="E76" s="109"/>
-      <c r="F76" s="111"/>
-      <c r="G76" s="111"/>
+      <c r="C76" s="118"/>
+      <c r="D76" s="107"/>
+      <c r="E76" s="108"/>
+      <c r="F76" s="110"/>
+      <c r="G76" s="110"/>
       <c r="H76" s="67"/>
       <c r="I76" s="1"/>
       <c r="J76" s="1"/>
@@ -32227,14 +32354,14 @@
     </row>
     <row r="77" ht="34.5" customHeight="1">
       <c r="A77" s="1"/>
-      <c r="B77" s="106">
+      <c r="B77" s="105">
         <v>5.0</v>
       </c>
-      <c r="C77" s="107"/>
-      <c r="D77" s="108"/>
-      <c r="E77" s="109"/>
-      <c r="F77" s="111"/>
-      <c r="G77" s="111"/>
+      <c r="C77" s="106"/>
+      <c r="D77" s="107"/>
+      <c r="E77" s="108"/>
+      <c r="F77" s="110"/>
+      <c r="G77" s="110"/>
       <c r="H77" s="67"/>
       <c r="I77" s="1"/>
       <c r="J77" s="1"/>
@@ -32257,14 +32384,14 @@
     </row>
     <row r="78" ht="34.5" customHeight="1">
       <c r="A78" s="1"/>
-      <c r="B78" s="114">
+      <c r="B78" s="113">
         <v>6.0</v>
       </c>
-      <c r="C78" s="107"/>
-      <c r="D78" s="115"/>
-      <c r="E78" s="109"/>
-      <c r="F78" s="111"/>
-      <c r="G78" s="111"/>
+      <c r="C78" s="106"/>
+      <c r="D78" s="114"/>
+      <c r="E78" s="108"/>
+      <c r="F78" s="110"/>
+      <c r="G78" s="110"/>
       <c r="H78" s="67"/>
       <c r="I78" s="1"/>
       <c r="J78" s="1"/>
@@ -32287,8 +32414,8 @@
     </row>
     <row r="79" ht="15.75" customHeight="1">
       <c r="A79" s="1"/>
-      <c r="B79" s="116"/>
-      <c r="C79" s="116"/>
+      <c r="B79" s="115"/>
+      <c r="C79" s="115"/>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
@@ -32315,14 +32442,14 @@
     </row>
     <row r="80" ht="15.75" customHeight="1">
       <c r="A80" s="1"/>
-      <c r="B80" s="118" t="s">
-        <v>48</v>
+      <c r="B80" s="117" t="s">
+        <v>53</v>
       </c>
-      <c r="C80" s="99"/>
-      <c r="D80" s="100"/>
-      <c r="E80" s="101"/>
-      <c r="F80" s="101"/>
-      <c r="G80" s="101"/>
+      <c r="C80" s="98"/>
+      <c r="D80" s="99"/>
+      <c r="E80" s="100"/>
+      <c r="F80" s="100"/>
+      <c r="G80" s="100"/>
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
       <c r="J80" s="1"/>
@@ -32345,23 +32472,23 @@
     </row>
     <row r="81" ht="18.0" customHeight="1">
       <c r="A81" s="1"/>
-      <c r="B81" s="102" t="s">
-        <v>52</v>
+      <c r="B81" s="101" t="s">
+        <v>59</v>
       </c>
-      <c r="C81" s="103" t="s">
-        <v>53</v>
+      <c r="C81" s="102" t="s">
+        <v>60</v>
       </c>
-      <c r="D81" s="103" t="s">
-        <v>54</v>
+      <c r="D81" s="102" t="s">
+        <v>61</v>
       </c>
-      <c r="E81" s="103" t="s">
-        <v>55</v>
+      <c r="E81" s="102" t="s">
+        <v>62</v>
       </c>
-      <c r="F81" s="104" t="s">
-        <v>56</v>
+      <c r="F81" s="103" t="s">
+        <v>63</v>
       </c>
-      <c r="G81" s="105" t="s">
-        <v>57</v>
+      <c r="G81" s="104" t="s">
+        <v>64</v>
       </c>
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
@@ -32385,14 +32512,20 @@
     </row>
     <row r="82" ht="34.5" customHeight="1">
       <c r="A82" s="1"/>
-      <c r="B82" s="106">
+      <c r="B82" s="105">
         <v>1.0</v>
       </c>
-      <c r="C82" s="107"/>
-      <c r="D82" s="108"/>
-      <c r="E82" s="109"/>
-      <c r="F82" s="111"/>
-      <c r="G82" s="111"/>
+      <c r="C82" s="111" t="s">
+        <v>85</v>
+      </c>
+      <c r="D82" s="107"/>
+      <c r="E82" s="112" t="s">
+        <v>86</v>
+      </c>
+      <c r="F82" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="G82" s="110"/>
       <c r="H82" s="67"/>
       <c r="I82" s="1"/>
       <c r="J82" s="1"/>
@@ -32415,14 +32548,22 @@
     </row>
     <row r="83" ht="34.5" customHeight="1">
       <c r="A83" s="1"/>
-      <c r="B83" s="106">
+      <c r="B83" s="105">
         <v>2.0</v>
       </c>
-      <c r="C83" s="107"/>
-      <c r="D83" s="108"/>
-      <c r="E83" s="109"/>
-      <c r="F83" s="111"/>
-      <c r="G83" s="111"/>
+      <c r="C83" s="111" t="s">
+        <v>87</v>
+      </c>
+      <c r="D83" s="107"/>
+      <c r="E83" s="112" t="s">
+        <v>88</v>
+      </c>
+      <c r="F83" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="G83" s="109" t="s">
+        <v>89</v>
+      </c>
       <c r="H83" s="67"/>
       <c r="I83" s="1"/>
       <c r="J83" s="1"/>
@@ -32445,14 +32586,20 @@
     </row>
     <row r="84" ht="34.5" customHeight="1">
       <c r="A84" s="1"/>
-      <c r="B84" s="106">
+      <c r="B84" s="105">
         <v>3.0</v>
       </c>
-      <c r="C84" s="107"/>
-      <c r="D84" s="108"/>
-      <c r="E84" s="109"/>
-      <c r="F84" s="111"/>
-      <c r="G84" s="111"/>
+      <c r="C84" s="111" t="s">
+        <v>90</v>
+      </c>
+      <c r="D84" s="107"/>
+      <c r="E84" s="112" t="s">
+        <v>91</v>
+      </c>
+      <c r="F84" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="G84" s="110"/>
       <c r="H84" s="67"/>
       <c r="I84" s="1"/>
       <c r="J84" s="1"/>
@@ -32475,14 +32622,20 @@
     </row>
     <row r="85" ht="34.5" customHeight="1">
       <c r="A85" s="1"/>
-      <c r="B85" s="106">
+      <c r="B85" s="105">
         <v>4.0</v>
       </c>
-      <c r="C85" s="119"/>
-      <c r="D85" s="108"/>
-      <c r="E85" s="109"/>
-      <c r="F85" s="111"/>
-      <c r="G85" s="111"/>
+      <c r="C85" s="111" t="s">
+        <v>87</v>
+      </c>
+      <c r="D85" s="107"/>
+      <c r="E85" s="112" t="s">
+        <v>92</v>
+      </c>
+      <c r="F85" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="G85" s="110"/>
       <c r="H85" s="67"/>
       <c r="I85" s="1"/>
       <c r="J85" s="1"/>
@@ -32505,14 +32658,14 @@
     </row>
     <row r="86" ht="34.5" customHeight="1">
       <c r="A86" s="1"/>
-      <c r="B86" s="106">
+      <c r="B86" s="105">
         <v>5.0</v>
       </c>
-      <c r="C86" s="107"/>
-      <c r="D86" s="108"/>
-      <c r="E86" s="109"/>
-      <c r="F86" s="111"/>
-      <c r="G86" s="111"/>
+      <c r="C86" s="106"/>
+      <c r="D86" s="107"/>
+      <c r="E86" s="108"/>
+      <c r="F86" s="110"/>
+      <c r="G86" s="110"/>
       <c r="H86" s="67"/>
       <c r="I86" s="1"/>
       <c r="J86" s="1"/>
@@ -32535,14 +32688,14 @@
     </row>
     <row r="87" ht="34.5" customHeight="1">
       <c r="A87" s="1"/>
-      <c r="B87" s="114">
+      <c r="B87" s="113">
         <v>6.0</v>
       </c>
-      <c r="C87" s="107"/>
-      <c r="D87" s="115"/>
-      <c r="E87" s="109"/>
-      <c r="F87" s="111"/>
-      <c r="G87" s="111"/>
+      <c r="C87" s="106"/>
+      <c r="D87" s="114"/>
+      <c r="E87" s="108"/>
+      <c r="F87" s="110"/>
+      <c r="G87" s="110"/>
       <c r="H87" s="67"/>
       <c r="I87" s="1"/>
       <c r="J87" s="1"/>
@@ -32565,8 +32718,8 @@
     </row>
     <row r="88" ht="15.75" customHeight="1">
       <c r="A88" s="1"/>
-      <c r="B88" s="116"/>
-      <c r="C88" s="116"/>
+      <c r="B88" s="115"/>
+      <c r="C88" s="115"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
@@ -32593,14 +32746,14 @@
     </row>
     <row r="89" ht="15.75" customHeight="1">
       <c r="A89" s="1"/>
-      <c r="B89" s="118" t="s">
-        <v>49</v>
+      <c r="B89" s="117" t="s">
+        <v>56</v>
       </c>
-      <c r="C89" s="99"/>
-      <c r="D89" s="100"/>
-      <c r="E89" s="101"/>
-      <c r="F89" s="101"/>
-      <c r="G89" s="101"/>
+      <c r="C89" s="98"/>
+      <c r="D89" s="99"/>
+      <c r="E89" s="100"/>
+      <c r="F89" s="100"/>
+      <c r="G89" s="100"/>
       <c r="H89" s="1"/>
       <c r="I89" s="1"/>
       <c r="J89" s="1"/>
@@ -32623,23 +32776,23 @@
     </row>
     <row r="90" ht="18.0" customHeight="1">
       <c r="A90" s="1"/>
-      <c r="B90" s="102" t="s">
-        <v>52</v>
+      <c r="B90" s="101" t="s">
+        <v>59</v>
       </c>
-      <c r="C90" s="103" t="s">
-        <v>53</v>
+      <c r="C90" s="102" t="s">
+        <v>60</v>
       </c>
-      <c r="D90" s="103" t="s">
-        <v>54</v>
+      <c r="D90" s="102" t="s">
+        <v>61</v>
       </c>
-      <c r="E90" s="103" t="s">
-        <v>55</v>
+      <c r="E90" s="102" t="s">
+        <v>62</v>
       </c>
-      <c r="F90" s="104" t="s">
-        <v>56</v>
+      <c r="F90" s="103" t="s">
+        <v>63</v>
       </c>
-      <c r="G90" s="105" t="s">
-        <v>57</v>
+      <c r="G90" s="104" t="s">
+        <v>64</v>
       </c>
       <c r="H90" s="1"/>
       <c r="I90" s="1"/>
@@ -32663,14 +32816,14 @@
     </row>
     <row r="91" ht="34.5" customHeight="1">
       <c r="A91" s="1"/>
-      <c r="B91" s="106">
+      <c r="B91" s="105">
         <v>1.0</v>
       </c>
-      <c r="C91" s="107"/>
-      <c r="D91" s="108"/>
-      <c r="E91" s="109"/>
-      <c r="F91" s="111"/>
-      <c r="G91" s="111"/>
+      <c r="C91" s="106"/>
+      <c r="D91" s="107"/>
+      <c r="E91" s="108"/>
+      <c r="F91" s="110"/>
+      <c r="G91" s="110"/>
       <c r="H91" s="67"/>
       <c r="I91" s="1"/>
       <c r="J91" s="1"/>
@@ -32693,14 +32846,14 @@
     </row>
     <row r="92" ht="34.5" customHeight="1">
       <c r="A92" s="1"/>
-      <c r="B92" s="106">
+      <c r="B92" s="105">
         <v>2.0</v>
       </c>
-      <c r="C92" s="107"/>
-      <c r="D92" s="108"/>
-      <c r="E92" s="109"/>
-      <c r="F92" s="111"/>
-      <c r="G92" s="111"/>
+      <c r="C92" s="106"/>
+      <c r="D92" s="107"/>
+      <c r="E92" s="108"/>
+      <c r="F92" s="110"/>
+      <c r="G92" s="110"/>
       <c r="H92" s="67"/>
       <c r="I92" s="1"/>
       <c r="J92" s="1"/>
@@ -32723,14 +32876,14 @@
     </row>
     <row r="93" ht="34.5" customHeight="1">
       <c r="A93" s="1"/>
-      <c r="B93" s="106">
+      <c r="B93" s="105">
         <v>3.0</v>
       </c>
-      <c r="C93" s="107"/>
-      <c r="D93" s="108"/>
-      <c r="E93" s="109"/>
-      <c r="F93" s="111"/>
-      <c r="G93" s="111"/>
+      <c r="C93" s="106"/>
+      <c r="D93" s="107"/>
+      <c r="E93" s="108"/>
+      <c r="F93" s="110"/>
+      <c r="G93" s="110"/>
       <c r="H93" s="67"/>
       <c r="I93" s="1"/>
       <c r="J93" s="1"/>
@@ -32753,14 +32906,14 @@
     </row>
     <row r="94" ht="34.5" customHeight="1">
       <c r="A94" s="1"/>
-      <c r="B94" s="106">
+      <c r="B94" s="105">
         <v>4.0</v>
       </c>
-      <c r="C94" s="119"/>
-      <c r="D94" s="108"/>
-      <c r="E94" s="109"/>
-      <c r="F94" s="111"/>
-      <c r="G94" s="111"/>
+      <c r="C94" s="118"/>
+      <c r="D94" s="107"/>
+      <c r="E94" s="108"/>
+      <c r="F94" s="110"/>
+      <c r="G94" s="110"/>
       <c r="H94" s="67"/>
       <c r="I94" s="1"/>
       <c r="J94" s="1"/>
@@ -32783,14 +32936,14 @@
     </row>
     <row r="95" ht="34.5" customHeight="1">
       <c r="A95" s="1"/>
-      <c r="B95" s="106">
+      <c r="B95" s="105">
         <v>5.0</v>
       </c>
-      <c r="C95" s="107"/>
-      <c r="D95" s="108"/>
-      <c r="E95" s="109"/>
-      <c r="F95" s="111"/>
-      <c r="G95" s="111"/>
+      <c r="C95" s="106"/>
+      <c r="D95" s="107"/>
+      <c r="E95" s="108"/>
+      <c r="F95" s="110"/>
+      <c r="G95" s="110"/>
       <c r="H95" s="67"/>
       <c r="I95" s="1"/>
       <c r="J95" s="1"/>
@@ -32813,14 +32966,14 @@
     </row>
     <row r="96" ht="34.5" customHeight="1">
       <c r="A96" s="1"/>
-      <c r="B96" s="114">
+      <c r="B96" s="113">
         <v>6.0</v>
       </c>
-      <c r="C96" s="107"/>
-      <c r="D96" s="115"/>
-      <c r="E96" s="109"/>
-      <c r="F96" s="111"/>
-      <c r="G96" s="111"/>
+      <c r="C96" s="106"/>
+      <c r="D96" s="114"/>
+      <c r="E96" s="108"/>
+      <c r="F96" s="110"/>
+      <c r="G96" s="110"/>
       <c r="H96" s="67"/>
       <c r="I96" s="1"/>
       <c r="J96" s="1"/>
@@ -32843,8 +32996,8 @@
     </row>
     <row r="97" ht="15.75" customHeight="1">
       <c r="A97" s="1"/>
-      <c r="B97" s="116"/>
-      <c r="C97" s="116"/>
+      <c r="B97" s="115"/>
+      <c r="C97" s="115"/>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
@@ -32871,14 +33024,14 @@
     </row>
     <row r="98" ht="15.75" customHeight="1">
       <c r="A98" s="1"/>
-      <c r="B98" s="118" t="s">
-        <v>50</v>
+      <c r="B98" s="117" t="s">
+        <v>57</v>
       </c>
-      <c r="C98" s="99"/>
-      <c r="D98" s="100"/>
-      <c r="E98" s="101"/>
-      <c r="F98" s="101"/>
-      <c r="G98" s="101"/>
+      <c r="C98" s="98"/>
+      <c r="D98" s="99"/>
+      <c r="E98" s="100"/>
+      <c r="F98" s="100"/>
+      <c r="G98" s="100"/>
       <c r="H98" s="1"/>
       <c r="I98" s="1"/>
       <c r="J98" s="1"/>
@@ -32901,23 +33054,23 @@
     </row>
     <row r="99" ht="18.0" customHeight="1">
       <c r="A99" s="1"/>
-      <c r="B99" s="102" t="s">
-        <v>52</v>
+      <c r="B99" s="101" t="s">
+        <v>59</v>
       </c>
-      <c r="C99" s="103" t="s">
-        <v>53</v>
+      <c r="C99" s="102" t="s">
+        <v>60</v>
       </c>
-      <c r="D99" s="103" t="s">
-        <v>54</v>
+      <c r="D99" s="102" t="s">
+        <v>61</v>
       </c>
-      <c r="E99" s="103" t="s">
-        <v>55</v>
+      <c r="E99" s="102" t="s">
+        <v>62</v>
       </c>
-      <c r="F99" s="104" t="s">
-        <v>56</v>
+      <c r="F99" s="103" t="s">
+        <v>63</v>
       </c>
-      <c r="G99" s="105" t="s">
-        <v>57</v>
+      <c r="G99" s="104" t="s">
+        <v>64</v>
       </c>
       <c r="H99" s="1"/>
       <c r="I99" s="1"/>
@@ -32941,14 +33094,14 @@
     </row>
     <row r="100" ht="34.5" customHeight="1">
       <c r="A100" s="1"/>
-      <c r="B100" s="106">
+      <c r="B100" s="105">
         <v>1.0</v>
       </c>
-      <c r="C100" s="107"/>
-      <c r="D100" s="108"/>
-      <c r="E100" s="109"/>
-      <c r="F100" s="111"/>
-      <c r="G100" s="111"/>
+      <c r="C100" s="106"/>
+      <c r="D100" s="107"/>
+      <c r="E100" s="108"/>
+      <c r="F100" s="110"/>
+      <c r="G100" s="110"/>
       <c r="H100" s="67"/>
       <c r="I100" s="1"/>
       <c r="J100" s="1"/>
@@ -32971,14 +33124,14 @@
     </row>
     <row r="101" ht="34.5" customHeight="1">
       <c r="A101" s="1"/>
-      <c r="B101" s="106">
+      <c r="B101" s="105">
         <v>2.0</v>
       </c>
-      <c r="C101" s="107"/>
-      <c r="D101" s="108"/>
-      <c r="E101" s="109"/>
-      <c r="F101" s="111"/>
-      <c r="G101" s="111"/>
+      <c r="C101" s="106"/>
+      <c r="D101" s="107"/>
+      <c r="E101" s="108"/>
+      <c r="F101" s="110"/>
+      <c r="G101" s="110"/>
       <c r="H101" s="67"/>
       <c r="I101" s="1"/>
       <c r="J101" s="1"/>
@@ -33001,14 +33154,14 @@
     </row>
     <row r="102" ht="34.5" customHeight="1">
       <c r="A102" s="1"/>
-      <c r="B102" s="106">
+      <c r="B102" s="105">
         <v>3.0</v>
       </c>
-      <c r="C102" s="107"/>
-      <c r="D102" s="108"/>
-      <c r="E102" s="109"/>
-      <c r="F102" s="111"/>
-      <c r="G102" s="111"/>
+      <c r="C102" s="106"/>
+      <c r="D102" s="107"/>
+      <c r="E102" s="108"/>
+      <c r="F102" s="110"/>
+      <c r="G102" s="110"/>
       <c r="H102" s="67"/>
       <c r="I102" s="1"/>
       <c r="J102" s="1"/>
@@ -33031,14 +33184,14 @@
     </row>
     <row r="103" ht="34.5" customHeight="1">
       <c r="A103" s="1"/>
-      <c r="B103" s="106">
+      <c r="B103" s="105">
         <v>4.0</v>
       </c>
-      <c r="C103" s="119"/>
-      <c r="D103" s="108"/>
-      <c r="E103" s="109"/>
-      <c r="F103" s="111"/>
-      <c r="G103" s="111"/>
+      <c r="C103" s="118"/>
+      <c r="D103" s="107"/>
+      <c r="E103" s="108"/>
+      <c r="F103" s="110"/>
+      <c r="G103" s="110"/>
       <c r="H103" s="67"/>
       <c r="I103" s="1"/>
       <c r="J103" s="1"/>
@@ -33061,14 +33214,14 @@
     </row>
     <row r="104" ht="34.5" customHeight="1">
       <c r="A104" s="1"/>
-      <c r="B104" s="106">
+      <c r="B104" s="105">
         <v>5.0</v>
       </c>
-      <c r="C104" s="107"/>
-      <c r="D104" s="108"/>
-      <c r="E104" s="109"/>
-      <c r="F104" s="111"/>
-      <c r="G104" s="111"/>
+      <c r="C104" s="106"/>
+      <c r="D104" s="107"/>
+      <c r="E104" s="108"/>
+      <c r="F104" s="110"/>
+      <c r="G104" s="110"/>
       <c r="H104" s="67"/>
       <c r="I104" s="1"/>
       <c r="J104" s="1"/>
@@ -33091,14 +33244,14 @@
     </row>
     <row r="105" ht="34.5" customHeight="1">
       <c r="A105" s="1"/>
-      <c r="B105" s="114">
+      <c r="B105" s="113">
         <v>6.0</v>
       </c>
-      <c r="C105" s="107"/>
-      <c r="D105" s="115"/>
-      <c r="E105" s="109"/>
-      <c r="F105" s="111"/>
-      <c r="G105" s="111"/>
+      <c r="C105" s="106"/>
+      <c r="D105" s="114"/>
+      <c r="E105" s="108"/>
+      <c r="F105" s="110"/>
+      <c r="G105" s="110"/>
       <c r="H105" s="67"/>
       <c r="I105" s="1"/>
       <c r="J105" s="1"/>
@@ -33121,8 +33274,8 @@
     </row>
     <row r="106" ht="15.75" customHeight="1">
       <c r="A106" s="1"/>
-      <c r="B106" s="116"/>
-      <c r="C106" s="116"/>
+      <c r="B106" s="115"/>
+      <c r="C106" s="115"/>
       <c r="D106" s="1"/>
       <c r="E106" s="1"/>
       <c r="F106" s="1"/>
@@ -33149,14 +33302,14 @@
     </row>
     <row r="107" ht="15.75" customHeight="1">
       <c r="A107" s="1"/>
-      <c r="B107" s="118" t="s">
-        <v>51</v>
+      <c r="B107" s="117" t="s">
+        <v>58</v>
       </c>
-      <c r="C107" s="99"/>
-      <c r="D107" s="100"/>
-      <c r="E107" s="101"/>
-      <c r="F107" s="101"/>
-      <c r="G107" s="101"/>
+      <c r="C107" s="98"/>
+      <c r="D107" s="99"/>
+      <c r="E107" s="100"/>
+      <c r="F107" s="100"/>
+      <c r="G107" s="100"/>
       <c r="H107" s="1"/>
       <c r="I107" s="1"/>
       <c r="J107" s="1"/>
@@ -33179,23 +33332,23 @@
     </row>
     <row r="108" ht="18.0" customHeight="1">
       <c r="A108" s="1"/>
-      <c r="B108" s="102" t="s">
-        <v>52</v>
+      <c r="B108" s="101" t="s">
+        <v>59</v>
       </c>
-      <c r="C108" s="103" t="s">
-        <v>53</v>
+      <c r="C108" s="102" t="s">
+        <v>60</v>
       </c>
-      <c r="D108" s="103" t="s">
-        <v>54</v>
+      <c r="D108" s="102" t="s">
+        <v>61</v>
       </c>
-      <c r="E108" s="103" t="s">
-        <v>55</v>
+      <c r="E108" s="102" t="s">
+        <v>62</v>
       </c>
-      <c r="F108" s="104" t="s">
-        <v>56</v>
+      <c r="F108" s="103" t="s">
+        <v>63</v>
       </c>
-      <c r="G108" s="105" t="s">
-        <v>57</v>
+      <c r="G108" s="104" t="s">
+        <v>64</v>
       </c>
       <c r="H108" s="1"/>
       <c r="I108" s="1"/>
@@ -33219,14 +33372,14 @@
     </row>
     <row r="109" ht="34.5" customHeight="1">
       <c r="A109" s="1"/>
-      <c r="B109" s="106">
+      <c r="B109" s="105">
         <v>1.0</v>
       </c>
-      <c r="C109" s="107"/>
-      <c r="D109" s="108"/>
-      <c r="E109" s="109"/>
-      <c r="F109" s="111"/>
-      <c r="G109" s="111"/>
+      <c r="C109" s="106"/>
+      <c r="D109" s="107"/>
+      <c r="E109" s="108"/>
+      <c r="F109" s="110"/>
+      <c r="G109" s="110"/>
       <c r="H109" s="67"/>
       <c r="I109" s="1"/>
       <c r="J109" s="1"/>
@@ -33249,14 +33402,14 @@
     </row>
     <row r="110" ht="34.5" customHeight="1">
       <c r="A110" s="1"/>
-      <c r="B110" s="106">
+      <c r="B110" s="105">
         <v>2.0</v>
       </c>
-      <c r="C110" s="107"/>
-      <c r="D110" s="108"/>
-      <c r="E110" s="109"/>
-      <c r="F110" s="111"/>
-      <c r="G110" s="111"/>
+      <c r="C110" s="106"/>
+      <c r="D110" s="107"/>
+      <c r="E110" s="108"/>
+      <c r="F110" s="110"/>
+      <c r="G110" s="110"/>
       <c r="H110" s="67"/>
       <c r="I110" s="1"/>
       <c r="J110" s="1"/>
@@ -33279,14 +33432,14 @@
     </row>
     <row r="111" ht="34.5" customHeight="1">
       <c r="A111" s="1"/>
-      <c r="B111" s="106">
+      <c r="B111" s="105">
         <v>3.0</v>
       </c>
-      <c r="C111" s="107"/>
-      <c r="D111" s="108"/>
-      <c r="E111" s="109"/>
-      <c r="F111" s="111"/>
-      <c r="G111" s="111"/>
+      <c r="C111" s="106"/>
+      <c r="D111" s="107"/>
+      <c r="E111" s="108"/>
+      <c r="F111" s="110"/>
+      <c r="G111" s="110"/>
       <c r="H111" s="67"/>
       <c r="I111" s="1"/>
       <c r="J111" s="1"/>
@@ -33309,14 +33462,14 @@
     </row>
     <row r="112" ht="34.5" customHeight="1">
       <c r="A112" s="1"/>
-      <c r="B112" s="106">
+      <c r="B112" s="105">
         <v>4.0</v>
       </c>
-      <c r="C112" s="119"/>
-      <c r="D112" s="108"/>
-      <c r="E112" s="109"/>
-      <c r="F112" s="111"/>
-      <c r="G112" s="111"/>
+      <c r="C112" s="118"/>
+      <c r="D112" s="107"/>
+      <c r="E112" s="108"/>
+      <c r="F112" s="110"/>
+      <c r="G112" s="110"/>
       <c r="H112" s="67"/>
       <c r="I112" s="1"/>
       <c r="J112" s="1"/>
@@ -33339,14 +33492,14 @@
     </row>
     <row r="113" ht="34.5" customHeight="1">
       <c r="A113" s="1"/>
-      <c r="B113" s="106">
+      <c r="B113" s="105">
         <v>5.0</v>
       </c>
-      <c r="C113" s="107"/>
-      <c r="D113" s="108"/>
-      <c r="E113" s="109"/>
-      <c r="F113" s="111"/>
-      <c r="G113" s="111"/>
+      <c r="C113" s="106"/>
+      <c r="D113" s="107"/>
+      <c r="E113" s="108"/>
+      <c r="F113" s="110"/>
+      <c r="G113" s="110"/>
       <c r="H113" s="67"/>
       <c r="I113" s="1"/>
       <c r="J113" s="1"/>
@@ -33369,14 +33522,14 @@
     </row>
     <row r="114" ht="34.5" customHeight="1">
       <c r="A114" s="1"/>
-      <c r="B114" s="114">
+      <c r="B114" s="113">
         <v>6.0</v>
       </c>
-      <c r="C114" s="107"/>
-      <c r="D114" s="115"/>
-      <c r="E114" s="109"/>
-      <c r="F114" s="111"/>
-      <c r="G114" s="111"/>
+      <c r="C114" s="106"/>
+      <c r="D114" s="114"/>
+      <c r="E114" s="108"/>
+      <c r="F114" s="110"/>
+      <c r="G114" s="110"/>
       <c r="H114" s="67"/>
       <c r="I114" s="1"/>
       <c r="J114" s="1"/>
@@ -58227,9 +58380,9 @@
     <mergeCell ref="F15:G15"/>
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F20:G20"/>
     <mergeCell ref="F18:G18"/>
     <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
     <mergeCell ref="B62:C62"/>
     <mergeCell ref="B71:C71"/>
     <mergeCell ref="B80:C80"/>

</xml_diff>